<commit_message>
modifie excel file creation future dont replace nan values with zeroes regenerate excel file with correct average scores by semester for subjects
</commit_message>
<xml_diff>
--- a/avg_subject_scores_by_semester.xlsx
+++ b/avg_subject_scores_by_semester.xlsx
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34.67957746478874</v>
+        <v>64.37254901960785</v>
       </c>
       <c r="D2" t="n">
-        <v>30.52992957746479</v>
+        <v>66.44061302681992</v>
       </c>
       <c r="E2" t="n">
-        <v>33.9031690140845</v>
+        <v>65.7235494880546</v>
       </c>
       <c r="F2" t="n">
-        <v>32.49471830985915</v>
+        <v>64.76140350877193</v>
       </c>
       <c r="G2" t="n">
-        <v>31.0862676056338</v>
+        <v>65.1549815498155</v>
       </c>
     </row>
     <row r="3">
@@ -505,19 +505,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30.38208409506398</v>
+        <v>65.68774703557312</v>
       </c>
       <c r="D3" t="n">
-        <v>29.80438756855576</v>
+        <v>63.18992248062015</v>
       </c>
       <c r="E3" t="n">
-        <v>30.85374771480804</v>
+        <v>64.66283524904215</v>
       </c>
       <c r="F3" t="n">
-        <v>32.26142595978062</v>
+        <v>64.87867647058823</v>
       </c>
       <c r="G3" t="n">
-        <v>31.74040219378428</v>
+        <v>63.13454545454545</v>
       </c>
     </row>
     <row r="4">
@@ -530,19 +530,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>33.16920473773266</v>
+        <v>64.06209150326798</v>
       </c>
       <c r="D4" t="n">
-        <v>32.20642978003384</v>
+        <v>65.18493150684931</v>
       </c>
       <c r="E4" t="n">
-        <v>33.91032148900169</v>
+        <v>65.70819672131148</v>
       </c>
       <c r="F4" t="n">
-        <v>32.75126903553299</v>
+        <v>63.46229508196721</v>
       </c>
       <c r="G4" t="n">
-        <v>32.99153976311337</v>
+        <v>66.77397260273973</v>
       </c>
     </row>
     <row r="5">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>35.63405797101449</v>
+        <v>66.45270270270271</v>
       </c>
       <c r="D5" t="n">
-        <v>30.17753623188406</v>
+        <v>64.31660231660231</v>
       </c>
       <c r="E5" t="n">
-        <v>34.39130434782609</v>
+        <v>64.79180887372014</v>
       </c>
       <c r="F5" t="n">
-        <v>32.15398550724638</v>
+        <v>64.77737226277372</v>
       </c>
       <c r="G5" t="n">
-        <v>33.90036231884058</v>
+        <v>64.30584192439862</v>
       </c>
     </row>
     <row r="6">
@@ -580,19 +580,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>35.86071428571429</v>
+        <v>63.55063291139241</v>
       </c>
       <c r="D6" t="n">
-        <v>32.70178571428571</v>
+        <v>65.17081850533808</v>
       </c>
       <c r="E6" t="n">
-        <v>30.83214285714286</v>
+        <v>64.90977443609023</v>
       </c>
       <c r="F6" t="n">
-        <v>33.98392857142857</v>
+        <v>66.07986111111111</v>
       </c>
       <c r="G6" t="n">
-        <v>33.22857142857143</v>
+        <v>65.06293706293707</v>
       </c>
     </row>
     <row r="7">
@@ -605,19 +605,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>33.55304347826087</v>
+        <v>63.8841059602649</v>
       </c>
       <c r="D7" t="n">
-        <v>31.29739130434783</v>
+        <v>65.67883211678833</v>
       </c>
       <c r="E7" t="n">
-        <v>34.14260869565217</v>
+        <v>66.32432432432432</v>
       </c>
       <c r="F7" t="n">
-        <v>32.12173913043478</v>
+        <v>66.67870036101083</v>
       </c>
       <c r="G7" t="n">
-        <v>33.34608695652174</v>
+        <v>64.55892255892256</v>
       </c>
     </row>
     <row r="8">
@@ -630,19 +630,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30.45026178010471</v>
+        <v>62.31428571428572</v>
       </c>
       <c r="D8" t="n">
-        <v>32.66317626527051</v>
+        <v>63.87713310580205</v>
       </c>
       <c r="E8" t="n">
-        <v>32.75741710296684</v>
+        <v>64.94809688581314</v>
       </c>
       <c r="F8" t="n">
-        <v>34.34031413612566</v>
+        <v>67.38698630136986</v>
       </c>
       <c r="G8" t="n">
-        <v>33.28272251308901</v>
+        <v>65.98961937716263</v>
       </c>
     </row>
     <row r="9">
@@ -655,19 +655,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>32.17465753424658</v>
+        <v>65.01730103806229</v>
       </c>
       <c r="D9" t="n">
-        <v>32.38013698630137</v>
+        <v>63.24414715719063</v>
       </c>
       <c r="E9" t="n">
-        <v>30.27739726027397</v>
+        <v>64.29818181818182</v>
       </c>
       <c r="F9" t="n">
-        <v>35.70376712328767</v>
+        <v>66.8301282051282</v>
       </c>
       <c r="G9" t="n">
-        <v>33.09075342465754</v>
+        <v>64.20265780730897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>